<commit_message>
translation system, db upload
</commit_message>
<xml_diff>
--- a/cityLife4/cityLifeDB.xlsx
+++ b/cityLife4/cityLifeDB.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="54">
   <si>
     <t>Apartments</t>
   </si>
@@ -91,6 +91,96 @@
   </si>
   <si>
     <t>/images/app2main.jpg</t>
+  </si>
+  <si>
+    <t>Languages</t>
+  </si>
+  <si>
+    <t>languageCode</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>isDefault</t>
+  </si>
+  <si>
+    <t>ru</t>
+  </si>
+  <si>
+    <t>Russian</t>
+  </si>
+  <si>
+    <t>true</t>
+  </si>
+  <si>
+    <t>en</t>
+  </si>
+  <si>
+    <t>English</t>
+  </si>
+  <si>
+    <t>false</t>
+  </si>
+  <si>
+    <t>isUsed</t>
+  </si>
+  <si>
+    <t>Translations</t>
+  </si>
+  <si>
+    <t>TranslationKeys</t>
+  </si>
+  <si>
+    <t>message</t>
+  </si>
+  <si>
+    <t>TranslationKey_id</t>
+  </si>
+  <si>
+    <t>Language_languageCode</t>
+  </si>
+  <si>
+    <t>Monday</t>
+  </si>
+  <si>
+    <t>Tuesday</t>
+  </si>
+  <si>
+    <t>Wednesday</t>
+  </si>
+  <si>
+    <t>creda</t>
+  </si>
+  <si>
+    <t>Thursday</t>
+  </si>
+  <si>
+    <t xml:space="preserve">thu   </t>
+  </si>
+  <si>
+    <t>chetverg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tue </t>
+  </si>
+  <si>
+    <t>home</t>
+  </si>
+  <si>
+    <t>booking</t>
+  </si>
+  <si>
+    <t>дом</t>
+  </si>
+  <si>
+    <t>Booking</t>
+  </si>
+  <si>
+    <t>букинг</t>
+  </si>
+  <si>
+    <t>transKey</t>
   </si>
 </sst>
 </file>
@@ -897,13 +987,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:I30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="18" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" customWidth="1"/>
     <col min="3" max="3" width="26.140625" customWidth="1"/>
+    <col min="4" max="4" width="20.42578125" customWidth="1"/>
+    <col min="5" max="5" width="17.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -1059,6 +1155,251 @@
         <v>2</v>
       </c>
     </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>36</v>
+      </c>
+      <c r="B14" t="s">
+        <v>1</v>
+      </c>
+      <c r="C14" t="s">
+        <v>53</v>
+      </c>
+      <c r="D14" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15" t="s">
+        <v>40</v>
+      </c>
+      <c r="D15" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B16">
+        <v>2</v>
+      </c>
+      <c r="C16" t="s">
+        <v>41</v>
+      </c>
+      <c r="D16" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B17">
+        <v>3</v>
+      </c>
+      <c r="C17" t="s">
+        <v>42</v>
+      </c>
+      <c r="D17" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B18">
+        <v>4</v>
+      </c>
+      <c r="C18" t="s">
+        <v>44</v>
+      </c>
+      <c r="D18" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B19">
+        <v>5</v>
+      </c>
+      <c r="C19" t="s">
+        <v>48</v>
+      </c>
+      <c r="D19" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B20">
+        <v>6</v>
+      </c>
+      <c r="C20" t="s">
+        <v>49</v>
+      </c>
+      <c r="D20" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>35</v>
+      </c>
+      <c r="B22" t="s">
+        <v>1</v>
+      </c>
+      <c r="C22" t="s">
+        <v>37</v>
+      </c>
+      <c r="D22" t="s">
+        <v>38</v>
+      </c>
+      <c r="E22" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="C23" t="s">
+        <v>47</v>
+      </c>
+      <c r="D23">
+        <v>2</v>
+      </c>
+      <c r="E23" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B24">
+        <v>2</v>
+      </c>
+      <c r="C24" t="s">
+        <v>43</v>
+      </c>
+      <c r="D24">
+        <v>3</v>
+      </c>
+      <c r="E24" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B25">
+        <v>3</v>
+      </c>
+      <c r="C25" t="s">
+        <v>45</v>
+      </c>
+      <c r="D25">
+        <v>4</v>
+      </c>
+      <c r="E25" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B26">
+        <v>4</v>
+      </c>
+      <c r="C26" t="s">
+        <v>46</v>
+      </c>
+      <c r="D26">
+        <v>4</v>
+      </c>
+      <c r="E26" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B27">
+        <v>5</v>
+      </c>
+      <c r="C27" t="s">
+        <v>48</v>
+      </c>
+      <c r="D27">
+        <v>5</v>
+      </c>
+      <c r="E27" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B28">
+        <v>6</v>
+      </c>
+      <c r="C28" t="s">
+        <v>50</v>
+      </c>
+      <c r="D28">
+        <v>5</v>
+      </c>
+      <c r="E28" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B29">
+        <v>7</v>
+      </c>
+      <c r="C29" t="s">
+        <v>51</v>
+      </c>
+      <c r="D29">
+        <v>6</v>
+      </c>
+      <c r="E29" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B30">
+        <v>8</v>
+      </c>
+      <c r="C30" t="s">
+        <v>52</v>
+      </c>
+      <c r="D30">
+        <v>6</v>
+      </c>
+      <c r="E30" t="s">
+        <v>28</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>